<commit_message>
3.1.5: Correct Path query.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTsResourceBundle.xlsx
+++ b/meta/program/BlancoRestGeneratorTsResourceBundle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97ED33AA-A3BA-4241-915C-02D71F59D3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6F9C93-0511-064C-A9C7-5F87554802E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20740" yWindow="9080" windowWidth="25520" windowHeight="12280" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="175">
   <si>
     <t>リソースバンドル定義書</t>
   </si>
@@ -950,6 +950,32 @@
     </rPh>
     <rPh sb="8" eb="9">
       <t xml:space="preserve">サイノ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>BLANCOREST.ERROR.MSG.07</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>クエリ種別Pathは必須です。[{0}] のパラメータ  [{1}] の設定を確認してください。</t>
+    <rPh sb="3" eb="5">
+      <t xml:space="preserve">シュベツ </t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">ヒッス </t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">イチラｎ </t>
+    </rPh>
+    <rPh sb="19" eb="29">
+      <t xml:space="preserve">セッテイヲ </t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t xml:space="preserve">カクニｎ </t>
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
@@ -1816,10 +1842,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -3106,7 +3132,7 @@
     </row>
     <row r="82" spans="1:8">
       <c r="A82" s="21">
-        <f t="shared" ref="A82:A114" si="1">A81+1</f>
+        <f t="shared" ref="A82:A115" si="1">A81+1</f>
         <v>68</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -3403,82 +3429,94 @@
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
+      <c r="B107" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="21">
-        <f t="shared" si="1"/>
-        <v>94</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>131</v>
+        <f>A106+1</f>
+        <v>93</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="21">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="21">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>95</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="21">
         <f t="shared" si="1"/>
-        <v>97</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>166</v>
+        <v>96</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="21">
         <f t="shared" si="1"/>
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="21">
         <f t="shared" si="1"/>
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="21">
         <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="21">
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3490,7 +3528,7 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D104:D106 D108:D109" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D109:D110 D104:D107" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>